<commit_message>
Added Movement Map Paradigm
</commit_message>
<xml_diff>
--- a/fMRI Tasks/info/biopac_code_dict.xlsx
+++ b/fMRI Tasks/info/biopac_code_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msun\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B5118E-803F-4485-A6D3-110ABF5D867E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7A7195-A354-4A20-B9D6-3DC5ED9A9D0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32070" yWindow="-23880" windowWidth="38640" windowHeight="23640" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="466">
   <si>
     <t>D8</t>
   </si>
@@ -1363,6 +1363,495 @@
   </si>
   <si>
     <t>audio100</t>
+  </si>
+  <si>
+    <r>
+      <t>movemapping_intro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>movement_instruction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>leftface_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>17</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rightface_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>leftarm_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rightarm_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>leftleg_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rightleg_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>chest_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>abdomen_cue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>leftface_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rightface_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>leftarm_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rightarm_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>28</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>leftleg_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>29</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rightleg_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>chest_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>abdomen_move</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>32</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>41</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>between_run_msg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>45</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>46</t>
+    </r>
+  </si>
+  <si>
+    <t>movemap</t>
+  </si>
+  <si>
+    <t>movementmap</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1861,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="########"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1401,8 +1890,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1412,6 +1919,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1E1E1E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1443,7 +1956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1477,6 +1990,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1794,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31222A2-51DB-244C-8B3D-C257DC9A15AB}">
   <dimension ref="A1:N268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2656,9 @@
       <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
@@ -9143,6 +9664,12 @@
       <c r="M156" s="2"/>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B157" s="12" t="s">
+        <v>443</v>
+      </c>
       <c r="C157" s="2">
         <v>155</v>
       </c>
@@ -9184,6 +9711,12 @@
       <c r="M157" s="2"/>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B158" s="12" t="s">
+        <v>444</v>
+      </c>
       <c r="C158" s="2">
         <v>156</v>
       </c>
@@ -9225,6 +9758,12 @@
       <c r="M158" s="2"/>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>445</v>
+      </c>
       <c r="C159" s="2">
         <v>157</v>
       </c>
@@ -9266,6 +9805,12 @@
       <c r="M159" s="2"/>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>446</v>
+      </c>
       <c r="C160" s="2">
         <v>158</v>
       </c>
@@ -9306,7 +9851,13 @@
       </c>
       <c r="M160" s="2"/>
     </row>
-    <row r="161" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B161" s="12" t="s">
+        <v>447</v>
+      </c>
       <c r="C161" s="2">
         <v>159</v>
       </c>
@@ -9347,7 +9898,13 @@
       </c>
       <c r="M161" s="2"/>
     </row>
-    <row r="162" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B162" s="12" t="s">
+        <v>448</v>
+      </c>
       <c r="C162" s="2">
         <v>160</v>
       </c>
@@ -9388,7 +9945,13 @@
       </c>
       <c r="M162" s="2"/>
     </row>
-    <row r="163" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B163" s="12" t="s">
+        <v>449</v>
+      </c>
       <c r="C163" s="2">
         <v>161</v>
       </c>
@@ -9429,7 +9992,13 @@
       </c>
       <c r="M163" s="2"/>
     </row>
-    <row r="164" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B164" s="12" t="s">
+        <v>450</v>
+      </c>
       <c r="C164" s="2">
         <v>162</v>
       </c>
@@ -9470,7 +10039,13 @@
       </c>
       <c r="M164" s="2"/>
     </row>
-    <row r="165" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B165" s="12" t="s">
+        <v>451</v>
+      </c>
       <c r="C165" s="2">
         <v>163</v>
       </c>
@@ -9511,7 +10086,13 @@
       </c>
       <c r="M165" s="2"/>
     </row>
-    <row r="166" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B166" s="12" t="s">
+        <v>452</v>
+      </c>
       <c r="C166" s="2">
         <v>164</v>
       </c>
@@ -9552,7 +10133,13 @@
       </c>
       <c r="M166" s="2"/>
     </row>
-    <row r="167" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B167" s="12" t="s">
+        <v>453</v>
+      </c>
       <c r="C167" s="2">
         <v>165</v>
       </c>
@@ -9593,7 +10180,13 @@
       </c>
       <c r="M167" s="2"/>
     </row>
-    <row r="168" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>454</v>
+      </c>
       <c r="C168" s="2">
         <v>166</v>
       </c>
@@ -9634,7 +10227,13 @@
       </c>
       <c r="M168" s="2"/>
     </row>
-    <row r="169" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B169" s="12" t="s">
+        <v>455</v>
+      </c>
       <c r="C169" s="2">
         <v>167</v>
       </c>
@@ -9675,7 +10274,13 @@
       </c>
       <c r="M169" s="2"/>
     </row>
-    <row r="170" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B170" s="12" t="s">
+        <v>456</v>
+      </c>
       <c r="C170" s="2">
         <v>168</v>
       </c>
@@ -9716,7 +10321,13 @@
       </c>
       <c r="M170" s="2"/>
     </row>
-    <row r="171" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B171" s="12" t="s">
+        <v>457</v>
+      </c>
       <c r="C171" s="2">
         <v>169</v>
       </c>
@@ -9757,7 +10368,13 @@
       </c>
       <c r="M171" s="2"/>
     </row>
-    <row r="172" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B172" s="12" t="s">
+        <v>458</v>
+      </c>
       <c r="C172" s="2">
         <v>170</v>
       </c>
@@ -9798,7 +10415,13 @@
       </c>
       <c r="M172" s="2"/>
     </row>
-    <row r="173" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B173" s="12" t="s">
+        <v>459</v>
+      </c>
       <c r="C173" s="2">
         <v>171</v>
       </c>
@@ -9839,7 +10462,13 @@
       </c>
       <c r="M173" s="2"/>
     </row>
-    <row r="174" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B174" s="12" t="s">
+        <v>460</v>
+      </c>
       <c r="C174" s="2">
         <v>172</v>
       </c>
@@ -9880,7 +10509,13 @@
       </c>
       <c r="M174" s="2"/>
     </row>
-    <row r="175" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B175" s="12" t="s">
+        <v>461</v>
+      </c>
       <c r="C175" s="2">
         <v>173</v>
       </c>
@@ -9921,7 +10556,13 @@
       </c>
       <c r="M175" s="2"/>
     </row>
-    <row r="176" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B176" s="12" t="s">
+        <v>462</v>
+      </c>
       <c r="C176" s="2">
         <v>174</v>
       </c>
@@ -9963,6 +10604,12 @@
       <c r="M176" s="2"/>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B177" s="12" t="s">
+        <v>463</v>
+      </c>
       <c r="C177" s="2">
         <v>175</v>
       </c>
@@ -10127,6 +10774,7 @@
       <c r="M180" s="2"/>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A181" s="13"/>
       <c r="C181" s="2">
         <v>179</v>
       </c>
@@ -10291,9 +10939,6 @@
       <c r="M184" s="2"/>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="B185" s="2"/>
       <c r="C185" s="2">
         <v>183</v>
@@ -13671,7 +14316,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="L2:L33 L34:L247" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Updated WASABI bodymap code to 2.0.0, Splitting imagination conditions into cue and orange fixation crosses
</commit_message>
<xml_diff>
--- a/fMRI Tasks/info/biopac_code_dict.xlsx
+++ b/fMRI Tasks/info/biopac_code_dict.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7A7195-A354-4A20-B9D6-3DC5ED9A9D0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EE35B2-50C0-4204-9ED1-1BE4FFD9700D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="38640" windowHeight="22650" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="472">
   <si>
     <t>D8</t>
   </si>
@@ -1365,493 +1365,91 @@
     <t>audio100</t>
   </si>
   <si>
-    <r>
-      <t>movemapping_intro</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>14</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>movement_instruction</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>leftface_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>17</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rightface_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>18</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>leftarm_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rightarm_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>leftleg_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>21</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rightleg_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>22</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>chest_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>23</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>abdomen_cue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>leftface_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rightface_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>leftarm_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rightarm_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>28</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>leftleg_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>29</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rightleg_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>30</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>chest_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>31</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>abdomen_move</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>32</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>41</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>between_run_msg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>45</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>end</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>46</t>
-    </r>
-  </si>
-  <si>
     <t>movemap</t>
   </si>
   <si>
     <t>movementmap</t>
+  </si>
+  <si>
+    <t>movemapping_intro</t>
+  </si>
+  <si>
+    <t>movement_instruction</t>
+  </si>
+  <si>
+    <t>leftface_cue</t>
+  </si>
+  <si>
+    <t>rightface_cue</t>
+  </si>
+  <si>
+    <t>leftarm_cue</t>
+  </si>
+  <si>
+    <t>rightarm_cue</t>
+  </si>
+  <si>
+    <t>leftleg_cue</t>
+  </si>
+  <si>
+    <t>rightleg_cue</t>
+  </si>
+  <si>
+    <t>chest_cue</t>
+  </si>
+  <si>
+    <t>abdomen_cue</t>
+  </si>
+  <si>
+    <t>leftface_move</t>
+  </si>
+  <si>
+    <t>rightface_move</t>
+  </si>
+  <si>
+    <t>leftarm_move</t>
+  </si>
+  <si>
+    <t>rightarm_move</t>
+  </si>
+  <si>
+    <t>leftleg_move</t>
+  </si>
+  <si>
+    <t>rightleg_move</t>
+  </si>
+  <si>
+    <t>chest_move</t>
+  </si>
+  <si>
+    <t>abdomen_move</t>
+  </si>
+  <si>
+    <t>between_run_msg</t>
+  </si>
+  <si>
+    <t>leftface_imagine_cue</t>
+  </si>
+  <si>
+    <t>rightface_imagine_cue</t>
+  </si>
+  <si>
+    <t>leftarm_imagine_cue</t>
+  </si>
+  <si>
+    <t>rightarm_imagine_cue</t>
+  </si>
+  <si>
+    <t>leftleg_imagine_cue</t>
+  </si>
+  <si>
+    <t>rightleg_imagine_cue</t>
+  </si>
+  <si>
+    <t>chest_imagine_cue</t>
+  </si>
+  <si>
+    <t>abdomen_imagine_cue</t>
   </si>
 </sst>
 </file>
@@ -1861,7 +1459,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="########"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1890,26 +1488,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFD4D4D4"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFB5CEA8"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1919,12 +1499,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1E1E1E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1956,7 +1530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1990,12 +1564,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2313,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31222A2-51DB-244C-8B3D-C257DC9A15AB}">
   <dimension ref="A1:N268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B194" sqref="B194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2657,7 +2225,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -9665,10 +9233,10 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B157" s="12" t="s">
-        <v>443</v>
+        <v>444</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>445</v>
       </c>
       <c r="C157" s="2">
         <v>155</v>
@@ -9712,10 +9280,10 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B158" s="12" t="s">
         <v>444</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>446</v>
       </c>
       <c r="C158" s="2">
         <v>156</v>
@@ -9759,10 +9327,10 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B159" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>447</v>
       </c>
       <c r="C159" s="2">
         <v>157</v>
@@ -9806,10 +9374,10 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B160" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>448</v>
       </c>
       <c r="C160" s="2">
         <v>158</v>
@@ -9853,10 +9421,10 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B161" s="12" t="s">
-        <v>447</v>
+        <v>444</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="C161" s="2">
         <v>159</v>
@@ -9900,10 +9468,10 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B162" s="12" t="s">
-        <v>448</v>
+        <v>444</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="C162" s="2">
         <v>160</v>
@@ -9947,10 +9515,10 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B163" s="12" t="s">
-        <v>449</v>
+        <v>444</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="C163" s="2">
         <v>161</v>
@@ -9994,10 +9562,10 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B164" s="12" t="s">
-        <v>450</v>
+        <v>444</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>452</v>
       </c>
       <c r="C164" s="2">
         <v>162</v>
@@ -10041,10 +9609,10 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B165" s="12" t="s">
-        <v>451</v>
+        <v>444</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="C165" s="2">
         <v>163</v>
@@ -10088,10 +9656,10 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B166" s="12" t="s">
-        <v>452</v>
+        <v>444</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>454</v>
       </c>
       <c r="C166" s="2">
         <v>164</v>
@@ -10135,10 +9703,10 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B167" s="12" t="s">
-        <v>453</v>
+        <v>444</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="C167" s="2">
         <v>165</v>
@@ -10182,10 +9750,10 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B168" s="12" t="s">
-        <v>454</v>
+        <v>444</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>456</v>
       </c>
       <c r="C168" s="2">
         <v>166</v>
@@ -10229,10 +9797,10 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B169" s="12" t="s">
-        <v>455</v>
+        <v>444</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>457</v>
       </c>
       <c r="C169" s="2">
         <v>167</v>
@@ -10276,10 +9844,10 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B170" s="12" t="s">
-        <v>456</v>
+        <v>444</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>458</v>
       </c>
       <c r="C170" s="2">
         <v>168</v>
@@ -10323,10 +9891,10 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B171" s="12" t="s">
-        <v>457</v>
+        <v>444</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>459</v>
       </c>
       <c r="C171" s="2">
         <v>169</v>
@@ -10370,10 +9938,10 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B172" s="12" t="s">
-        <v>458</v>
+        <v>444</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>460</v>
       </c>
       <c r="C172" s="2">
         <v>170</v>
@@ -10417,10 +9985,10 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B173" s="12" t="s">
-        <v>459</v>
+        <v>444</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>461</v>
       </c>
       <c r="C173" s="2">
         <v>171</v>
@@ -10464,10 +10032,10 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B174" s="12" t="s">
-        <v>460</v>
+        <v>444</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>462</v>
       </c>
       <c r="C174" s="2">
         <v>172</v>
@@ -10511,10 +10079,10 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B175" s="12" t="s">
-        <v>461</v>
+        <v>444</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>330</v>
       </c>
       <c r="C175" s="2">
         <v>173</v>
@@ -10558,10 +10126,10 @@
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B176" s="12" t="s">
-        <v>462</v>
+        <v>444</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>463</v>
       </c>
       <c r="C176" s="2">
         <v>174</v>
@@ -10605,10 +10173,10 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B177" s="12" t="s">
-        <v>463</v>
+        <v>444</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="C177" s="2">
         <v>175</v>
@@ -10651,6 +10219,12 @@
       <c r="M177" s="2"/>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A178" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>464</v>
+      </c>
       <c r="C178" s="2">
         <v>176</v>
       </c>
@@ -10692,6 +10266,12 @@
       <c r="M178" s="2"/>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A179" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>465</v>
+      </c>
       <c r="C179" s="2">
         <v>177</v>
       </c>
@@ -10733,6 +10313,12 @@
       <c r="M179" s="2"/>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A180" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>466</v>
+      </c>
       <c r="C180" s="2">
         <v>178</v>
       </c>
@@ -10774,7 +10360,12 @@
       <c r="M180" s="2"/>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A181" s="13"/>
+      <c r="A181" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>467</v>
+      </c>
       <c r="C181" s="2">
         <v>179</v>
       </c>
@@ -10816,6 +10407,12 @@
       <c r="M181" s="2"/>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A182" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>468</v>
+      </c>
       <c r="C182" s="2">
         <v>180</v>
       </c>
@@ -10857,6 +10454,12 @@
       <c r="M182" s="2"/>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A183" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>469</v>
+      </c>
       <c r="C183" s="2">
         <v>181</v>
       </c>
@@ -10898,6 +10501,12 @@
       <c r="M183" s="2"/>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A184" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>470</v>
+      </c>
       <c r="C184" s="2">
         <v>182</v>
       </c>
@@ -10939,7 +10548,12 @@
       <c r="M184" s="2"/>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B185" s="2"/>
+      <c r="A185" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>471</v>
+      </c>
       <c r="C185" s="2">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
First push of kungfury-hyperalignment paradigm
</commit_message>
<xml_diff>
--- a/fMRI Tasks/info/biopac_code_dict.xlsx
+++ b/fMRI Tasks/info/biopac_code_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EE35B2-50C0-4204-9ED1-1BE4FFD9700D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1120A680-DC29-4F96-BE47-1A7F822FD043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="38640" windowHeight="22650" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="472">
   <si>
     <t>D8</t>
   </si>
@@ -864,18 +864,6 @@
     <t>intro</t>
   </si>
   <si>
-    <t>video_start</t>
-  </si>
-  <si>
-    <t>video_end</t>
-  </si>
-  <si>
-    <t>rating_start</t>
-  </si>
-  <si>
-    <t>rating_end</t>
-  </si>
-  <si>
     <t>rating order: personal relevance, happy, sad, afraid, disgusted, warm and tender, engaged</t>
   </si>
   <si>
@@ -1450,6 +1438,18 @@
   </si>
   <si>
     <t>abdomen_imagine_cue</t>
+  </si>
+  <si>
+    <t>kungfury</t>
+  </si>
+  <si>
+    <t>inscapes</t>
+  </si>
+  <si>
+    <t>resting_state</t>
+  </si>
+  <si>
+    <t>hyperalignment_intro</t>
   </si>
 </sst>
 </file>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31222A2-51DB-244C-8B3D-C257DC9A15AB}">
   <dimension ref="A1:N268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="B194" sqref="B194"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1937,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>13</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>13</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>13</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>13</v>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -2372,7 +2372,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C11" s="2">
         <v>9</v>
@@ -2420,7 +2420,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C12" s="2">
         <v>10</v>
@@ -2468,7 +2468,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C13" s="2">
         <v>11</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>275</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C17" s="2">
         <v>15</v>
@@ -2701,10 +2701,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C18" s="2">
         <v>16</v>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C19" s="2">
         <v>17</v>
@@ -2795,10 +2795,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C20" s="2">
         <v>18</v>
@@ -2842,10 +2842,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C21" s="2">
         <v>19</v>
@@ -2889,10 +2889,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C22" s="2">
         <v>20</v>
@@ -2936,10 +2936,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C23" s="2">
         <v>21</v>
@@ -2983,10 +2983,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C24" s="2">
         <v>22</v>
@@ -3030,10 +3030,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C25" s="2">
         <v>23</v>
@@ -3077,10 +3077,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C26" s="2">
         <v>24</v>
@@ -3124,10 +3124,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C27" s="2">
         <v>25</v>
@@ -3171,10 +3171,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C28" s="2">
         <v>26</v>
@@ -3218,10 +3218,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C29" s="2">
         <v>27</v>
@@ -3265,10 +3265,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C30" s="2">
         <v>28</v>
@@ -3312,10 +3312,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C31" s="2">
         <v>29</v>
@@ -3359,10 +3359,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C32" s="2">
         <v>30</v>
@@ -3406,10 +3406,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C33" s="2">
         <v>31</v>
@@ -3453,10 +3453,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C34" s="2">
         <v>32</v>
@@ -3500,10 +3500,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C35" s="2">
         <v>33</v>
@@ -3547,10 +3547,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C36" s="2">
         <v>34</v>
@@ -3594,10 +3594,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C37" s="2">
         <v>35</v>
@@ -3641,10 +3641,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C38" s="2">
         <v>36</v>
@@ -3688,10 +3688,10 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C39" s="2">
         <v>37</v>
@@ -3735,10 +3735,10 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C40" s="2">
         <v>38</v>
@@ -3782,10 +3782,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C41" s="2">
         <v>39</v>
@@ -3829,10 +3829,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C42" s="2">
         <v>40</v>
@@ -3876,10 +3876,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C43" s="2">
         <v>41</v>
@@ -3923,10 +3923,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C44" s="2">
         <v>42</v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C45" s="2">
         <v>43</v>
@@ -4017,10 +4017,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C46" s="2">
         <v>44</v>
@@ -4064,10 +4064,10 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C47" s="2">
         <v>45</v>
@@ -4111,10 +4111,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C48" s="2">
         <v>46</v>
@@ -4158,10 +4158,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C49" s="2">
         <v>47</v>
@@ -4205,10 +4205,10 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C50" s="2">
         <v>48</v>
@@ -4252,10 +4252,10 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C51" s="2">
         <v>49</v>
@@ -4299,10 +4299,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C52" s="2">
         <v>50</v>
@@ -4346,10 +4346,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C53" s="2">
         <v>51</v>
@@ -4393,10 +4393,10 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C54" s="2">
         <v>52</v>
@@ -4440,10 +4440,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C55" s="2">
         <v>53</v>
@@ -4487,10 +4487,10 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C56" s="2">
         <v>54</v>
@@ -4534,10 +4534,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>344</v>
       </c>
       <c r="C57" s="2">
         <v>55</v>
@@ -4581,10 +4581,10 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C58" s="2">
         <v>56</v>
@@ -4628,10 +4628,10 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C59" s="2">
         <v>57</v>
@@ -4675,10 +4675,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C60" s="2">
         <v>58</v>
@@ -4722,10 +4722,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C61" s="2">
         <v>59</v>
@@ -4769,10 +4769,10 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C62" s="2">
         <v>60</v>
@@ -4816,10 +4816,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C63" s="2">
         <v>61</v>
@@ -4863,10 +4863,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C64" s="2">
         <v>62</v>
@@ -4910,10 +4910,10 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C65" s="2">
         <v>63</v>
@@ -4957,10 +4957,10 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C66" s="2">
         <v>64</v>
@@ -5004,10 +5004,10 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C67" s="2">
         <v>65</v>
@@ -5051,10 +5051,10 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C68" s="2">
         <v>66</v>
@@ -5098,10 +5098,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C69" s="2">
         <v>67</v>
@@ -5145,10 +5145,10 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C70" s="2">
         <v>68</v>
@@ -5192,10 +5192,10 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C71" s="2">
         <v>69</v>
@@ -5239,10 +5239,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C72" s="2">
         <v>70</v>
@@ -5286,10 +5286,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C73" s="2">
         <v>71</v>
@@ -5333,10 +5333,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C74" s="2">
         <v>72</v>
@@ -5380,10 +5380,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C75" s="2">
         <v>73</v>
@@ -5427,10 +5427,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C76" s="2">
         <v>74</v>
@@ -5474,10 +5474,10 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C77" s="2">
         <v>75</v>
@@ -5521,10 +5521,10 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C78" s="2">
         <v>76</v>
@@ -5568,10 +5568,10 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C79" s="2">
         <v>77</v>
@@ -5615,10 +5615,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C80" s="2">
         <v>78</v>
@@ -5662,10 +5662,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C81" s="2">
         <v>79</v>
@@ -5709,10 +5709,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C82" s="2">
         <v>80</v>
@@ -5756,10 +5756,10 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C83" s="2">
         <v>81</v>
@@ -5803,10 +5803,10 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C84" s="2">
         <v>82</v>
@@ -5850,10 +5850,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C85" s="2">
         <v>83</v>
@@ -5897,10 +5897,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C86" s="2">
         <v>84</v>
@@ -5944,10 +5944,10 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C87" s="2">
         <v>85</v>
@@ -5991,10 +5991,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C88" s="2">
         <v>86</v>
@@ -6038,10 +6038,10 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C89" s="2">
         <v>87</v>
@@ -6085,10 +6085,10 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C90" s="2">
         <v>88</v>
@@ -6132,10 +6132,10 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C91" s="2">
         <v>89</v>
@@ -6179,10 +6179,10 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C92" s="2">
         <v>90</v>
@@ -6226,10 +6226,10 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C93" s="2">
         <v>91</v>
@@ -6273,10 +6273,10 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C94" s="2">
         <v>92</v>
@@ -6320,10 +6320,10 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C95" s="2">
         <v>93</v>
@@ -6367,10 +6367,10 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C96" s="2">
         <v>94</v>
@@ -6414,10 +6414,10 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C97" s="2">
         <v>95</v>
@@ -6461,10 +6461,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C98" s="2">
         <v>96</v>
@@ -6508,10 +6508,10 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C99" s="2">
         <v>97</v>
@@ -6555,10 +6555,10 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C100" s="2">
         <v>98</v>
@@ -6602,10 +6602,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C101" s="2">
         <v>99</v>
@@ -6649,10 +6649,10 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C102" s="2">
         <v>100</v>
@@ -6696,10 +6696,10 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C103" s="2">
         <v>101</v>
@@ -6743,10 +6743,10 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C104" s="2">
         <v>102</v>
@@ -6790,10 +6790,10 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C105" s="2">
         <v>103</v>
@@ -6836,10 +6836,10 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C106" s="2">
         <v>104</v>
@@ -6883,10 +6883,10 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C107" s="2">
         <v>105</v>
@@ -6930,10 +6930,10 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C108" s="2">
         <v>106</v>
@@ -6977,10 +6977,10 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C109" s="2">
         <v>107</v>
@@ -7024,10 +7024,10 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C110" s="2">
         <v>108</v>
@@ -7071,10 +7071,10 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C111" s="2">
         <v>109</v>
@@ -7118,10 +7118,10 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C112" s="2">
         <v>110</v>
@@ -7165,10 +7165,10 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C113" s="2">
         <v>111</v>
@@ -7212,10 +7212,10 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C114" s="2">
         <v>112</v>
@@ -7259,10 +7259,10 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C115" s="2">
         <v>113</v>
@@ -7306,10 +7306,10 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C116" s="2">
         <v>114</v>
@@ -7353,10 +7353,10 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C117" s="2">
         <v>115</v>
@@ -7400,10 +7400,10 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C118" s="2">
         <v>116</v>
@@ -7447,10 +7447,10 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C119" s="2">
         <v>117</v>
@@ -7494,10 +7494,10 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C120" s="2">
         <v>118</v>
@@ -7541,10 +7541,10 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C121" s="2">
         <v>119</v>
@@ -7588,10 +7588,10 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C122" s="2">
         <v>120</v>
@@ -7635,10 +7635,10 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C123" s="2">
         <v>121</v>
@@ -7682,10 +7682,10 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C124" s="2">
         <v>122</v>
@@ -7729,10 +7729,10 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C125" s="2">
         <v>123</v>
@@ -7776,10 +7776,10 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C126" s="2">
         <v>124</v>
@@ -7823,10 +7823,10 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C127" s="2">
         <v>125</v>
@@ -7870,10 +7870,10 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C128" s="2">
         <v>126</v>
@@ -7917,10 +7917,10 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C129" s="2">
         <v>127</v>
@@ -7964,10 +7964,10 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C130" s="2">
         <v>128</v>
@@ -8011,10 +8011,10 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C131" s="2">
         <v>129</v>
@@ -8058,10 +8058,10 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C132" s="2">
         <v>130</v>
@@ -8105,10 +8105,10 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C133" s="2">
         <v>131</v>
@@ -8152,10 +8152,10 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C134" s="2">
         <v>132</v>
@@ -8199,10 +8199,10 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C135" s="2">
         <v>133</v>
@@ -8246,10 +8246,10 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C136" s="2">
         <v>134</v>
@@ -8293,10 +8293,10 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C137" s="2">
         <v>135</v>
@@ -8340,10 +8340,10 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C138" s="2">
         <v>136</v>
@@ -8387,10 +8387,10 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C139" s="2">
         <v>137</v>
@@ -8434,10 +8434,10 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C140" s="2">
         <v>138</v>
@@ -8481,10 +8481,10 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C141" s="2">
         <v>139</v>
@@ -8528,10 +8528,10 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C142" s="2">
         <v>140</v>
@@ -8575,10 +8575,10 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C143" s="2">
         <v>141</v>
@@ -8622,10 +8622,10 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C144" s="2">
         <v>142</v>
@@ -8669,10 +8669,10 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C145" s="2">
         <v>143</v>
@@ -8716,10 +8716,10 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C146" s="2">
         <v>144</v>
@@ -8763,10 +8763,10 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C147" s="2">
         <v>145</v>
@@ -8810,10 +8810,10 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C148" s="2">
         <v>146</v>
@@ -8857,10 +8857,10 @@
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C149" s="2">
         <v>147</v>
@@ -8904,10 +8904,10 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C150" s="2">
         <v>148</v>
@@ -8951,10 +8951,10 @@
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C151" s="2">
         <v>149</v>
@@ -8998,10 +8998,10 @@
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C152" s="2">
         <v>150</v>
@@ -9045,10 +9045,10 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C153" s="2">
         <v>151</v>
@@ -9092,10 +9092,10 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C154" s="2">
         <v>152</v>
@@ -9139,10 +9139,10 @@
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C155" s="2">
         <v>153</v>
@@ -9186,10 +9186,10 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C156" s="2">
         <v>154</v>
@@ -9233,10 +9233,10 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C157" s="2">
         <v>155</v>
@@ -9280,10 +9280,10 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C158" s="2">
         <v>156</v>
@@ -9327,10 +9327,10 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C159" s="2">
         <v>157</v>
@@ -9374,10 +9374,10 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B160" s="3" t="s">
         <v>444</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>448</v>
       </c>
       <c r="C160" s="2">
         <v>158</v>
@@ -9421,10 +9421,10 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C161" s="2">
         <v>159</v>
@@ -9468,10 +9468,10 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C162" s="2">
         <v>160</v>
@@ -9515,10 +9515,10 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C163" s="2">
         <v>161</v>
@@ -9562,10 +9562,10 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C164" s="2">
         <v>162</v>
@@ -9609,10 +9609,10 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C165" s="2">
         <v>163</v>
@@ -9656,10 +9656,10 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C166" s="2">
         <v>164</v>
@@ -9703,10 +9703,10 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C167" s="2">
         <v>165</v>
@@ -9750,10 +9750,10 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C168" s="2">
         <v>166</v>
@@ -9797,10 +9797,10 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C169" s="2">
         <v>167</v>
@@ -9844,10 +9844,10 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C170" s="2">
         <v>168</v>
@@ -9891,10 +9891,10 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C171" s="2">
         <v>169</v>
@@ -9938,10 +9938,10 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C172" s="2">
         <v>170</v>
@@ -9985,10 +9985,10 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C173" s="2">
         <v>171</v>
@@ -10032,10 +10032,10 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C174" s="2">
         <v>172</v>
@@ -10079,10 +10079,10 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C175" s="2">
         <v>173</v>
@@ -10126,10 +10126,10 @@
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C176" s="2">
         <v>174</v>
@@ -10173,10 +10173,10 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C177" s="2">
         <v>175</v>
@@ -10220,10 +10220,10 @@
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C178" s="2">
         <v>176</v>
@@ -10267,10 +10267,10 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C179" s="2">
         <v>177</v>
@@ -10314,10 +10314,10 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C180" s="2">
         <v>178</v>
@@ -10361,10 +10361,10 @@
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C181" s="2">
         <v>179</v>
@@ -10408,10 +10408,10 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C182" s="2">
         <v>180</v>
@@ -10455,10 +10455,10 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C183" s="2">
         <v>181</v>
@@ -10502,10 +10502,10 @@
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C184" s="2">
         <v>182</v>
@@ -10549,10 +10549,10 @@
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C185" s="2">
         <v>183</v>
@@ -10596,7 +10596,7 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B186" s="10" t="s">
         <v>275</v>
@@ -10643,10 +10643,10 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C187" s="2">
         <v>185</v>
@@ -10690,10 +10690,10 @@
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C188" s="2">
         <v>186</v>
@@ -10737,10 +10737,10 @@
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C189" s="2">
         <v>187</v>
@@ -10784,10 +10784,10 @@
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B190" s="8" t="s">
         <v>333</v>
-      </c>
-      <c r="B190" s="8" t="s">
-        <v>337</v>
       </c>
       <c r="C190" s="2">
         <v>188</v>
@@ -10831,10 +10831,10 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C191" s="2">
         <v>189</v>
@@ -10878,10 +10878,10 @@
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C192" s="2">
         <v>190</v>
@@ -10925,10 +10925,10 @@
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C193" s="2">
         <v>191</v>
@@ -10972,10 +10972,10 @@
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C194" s="2">
         <v>192</v>
@@ -11244,10 +11244,10 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C200" s="2">
         <v>198</v>
@@ -11291,10 +11291,10 @@
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C201" s="2">
         <v>199</v>
@@ -11338,10 +11338,10 @@
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C202" s="2">
         <v>200</v>
@@ -11385,10 +11385,10 @@
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C203" s="2">
         <v>201</v>
@@ -11432,10 +11432,10 @@
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C204" s="2">
         <v>202</v>
@@ -11479,10 +11479,10 @@
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C205" s="2">
         <v>203</v>
@@ -11526,10 +11526,10 @@
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C206" s="2">
         <v>204</v>
@@ -11573,10 +11573,10 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C207" s="2">
         <v>205</v>
@@ -11620,10 +11620,10 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C208" s="2">
         <v>206</v>
@@ -11667,10 +11667,10 @@
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C209" s="2">
         <v>207</v>
@@ -11714,10 +11714,10 @@
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C210" s="2">
         <v>208</v>
@@ -11761,10 +11761,10 @@
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C211" s="2">
         <v>209</v>
@@ -11808,10 +11808,10 @@
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C212" s="2">
         <v>210</v>
@@ -11855,10 +11855,10 @@
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C213" s="2">
         <v>211</v>
@@ -11902,10 +11902,10 @@
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="B214" s="8" t="s">
-        <v>13</v>
+        <v>295</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>471</v>
       </c>
       <c r="C214" s="2">
         <v>212</v>
@@ -11949,10 +11949,10 @@
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" s="8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>276</v>
+        <v>468</v>
       </c>
       <c r="C215" s="2">
         <v>213</v>
@@ -11996,10 +11996,10 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" s="8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>277</v>
+        <v>469</v>
       </c>
       <c r="C216" s="2">
         <v>214</v>
@@ -12043,10 +12043,10 @@
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" s="8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>278</v>
+        <v>470</v>
       </c>
       <c r="C217" s="2">
         <v>215</v>
@@ -12087,15 +12087,12 @@
         <v>229</v>
       </c>
       <c r="M217" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A218" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="B218" s="8" t="s">
-        <v>279</v>
+      <c r="A218" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C218" s="2">
         <v>216</v>

</xml_diff>

<commit_message>
Code cleanup and first release of distractmap v1.0.0
</commit_message>
<xml_diff>
--- a/fMRI Tasks/info/biopac_code_dict.xlsx
+++ b/fMRI Tasks/info/biopac_code_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1120A680-DC29-4F96-BE47-1A7F822FD043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C4FA63-28BA-42AE-A310-3109ABD91141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
+    <workbookView xWindow="38280" yWindow="285" windowWidth="38640" windowHeight="22650" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="473">
   <si>
     <t>D8</t>
   </si>
@@ -846,18 +846,6 @@
     <t>11111111</t>
   </si>
   <si>
-    <t>task_start</t>
-  </si>
-  <si>
-    <t>task_end</t>
-  </si>
-  <si>
-    <t>trial_start</t>
-  </si>
-  <si>
-    <t>trial_end</t>
-  </si>
-  <si>
     <t>baseline</t>
   </si>
   <si>
@@ -924,15 +912,6 @@
     <t>hyperalignment</t>
   </si>
   <si>
-    <t>run_start</t>
-  </si>
-  <si>
-    <t>run_end</t>
-  </si>
-  <si>
-    <t>run_middle</t>
-  </si>
-  <si>
     <t>leftface_heat_start</t>
   </si>
   <si>
@@ -1450,6 +1429,30 @@
   </si>
   <si>
     <t>hyperalignment_intro</t>
+  </si>
+  <si>
+    <t>distractmap</t>
+  </si>
+  <si>
+    <t>acceptmap</t>
+  </si>
+  <si>
+    <t>nback_feedback_pos</t>
+  </si>
+  <si>
+    <t>nback_feedback_miss</t>
+  </si>
+  <si>
+    <t>nback_feedback_neg</t>
+  </si>
+  <si>
+    <t>t1_test/distractmap</t>
+  </si>
+  <si>
+    <t>bodymapping/distractmap</t>
+  </si>
+  <si>
+    <t>bodymapping_instruction</t>
   </si>
 </sst>
 </file>
@@ -1881,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31222A2-51DB-244C-8B3D-C257DC9A15AB}">
   <dimension ref="A1:N268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="B217" sqref="B217"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="E208" sqref="E208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1937,15 +1940,15 @@
         <v>9</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1989,7 +1992,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>13</v>
@@ -2036,7 +2039,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>13</v>
@@ -2083,7 +2086,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>13</v>
@@ -2130,7 +2133,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>13</v>
@@ -2177,7 +2180,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>294</v>
+        <v>465</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
@@ -2225,7 +2228,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -2273,10 +2276,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>12</v>
+        <v>466</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>270</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2">
         <v>7</v>
@@ -2320,12 +2323,8 @@
       <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>271</v>
-      </c>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="2">
         <v>8</v>
       </c>
@@ -2368,12 +2367,8 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>296</v>
-      </c>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2">
         <v>9</v>
       </c>
@@ -2416,12 +2411,8 @@
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>297</v>
-      </c>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2">
         <v>10</v>
       </c>
@@ -2464,12 +2455,8 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>298</v>
-      </c>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2">
         <v>11</v>
       </c>
@@ -2512,12 +2499,8 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>272</v>
-      </c>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="2">
         <v>12</v>
       </c>
@@ -2559,12 +2542,8 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>273</v>
-      </c>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="2">
         <v>13</v>
       </c>
@@ -2607,10 +2586,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C16" s="2">
         <v>14</v>
@@ -2653,11 +2632,11 @@
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>292</v>
+      <c r="A17" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>472</v>
       </c>
       <c r="C17" s="2">
         <v>15</v>
@@ -2701,10 +2680,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C18" s="2">
         <v>16</v>
@@ -2748,10 +2727,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>293</v>
+        <v>471</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C19" s="2">
         <v>17</v>
@@ -2795,10 +2774,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>301</v>
       </c>
       <c r="C20" s="2">
         <v>18</v>
@@ -2842,10 +2821,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>293</v>
+        <v>471</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C21" s="2">
         <v>19</v>
@@ -2889,10 +2868,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>293</v>
+        <v>471</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C22" s="2">
         <v>20</v>
@@ -2936,10 +2915,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>293</v>
+        <v>471</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C23" s="2">
         <v>21</v>
@@ -2983,10 +2962,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>293</v>
+        <v>471</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C24" s="2">
         <v>22</v>
@@ -3030,10 +3009,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>293</v>
+        <v>471</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C25" s="2">
         <v>23</v>
@@ -3077,10 +3056,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>293</v>
+        <v>471</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C26" s="2">
         <v>24</v>
@@ -3124,10 +3103,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C27" s="2">
         <v>25</v>
@@ -3171,10 +3150,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C28" s="2">
         <v>26</v>
@@ -3218,10 +3197,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C29" s="2">
         <v>27</v>
@@ -3265,10 +3244,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C30" s="2">
         <v>28</v>
@@ -3312,10 +3291,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C31" s="2">
         <v>29</v>
@@ -3359,10 +3338,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C32" s="2">
         <v>30</v>
@@ -3406,10 +3385,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C33" s="2">
         <v>31</v>
@@ -3453,10 +3432,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C34" s="2">
         <v>32</v>
@@ -3500,10 +3479,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C35" s="2">
         <v>33</v>
@@ -3547,10 +3526,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C36" s="2">
         <v>34</v>
@@ -3594,10 +3573,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C37" s="2">
         <v>35</v>
@@ -3641,10 +3620,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C38" s="2">
         <v>36</v>
@@ -3688,10 +3667,10 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C39" s="2">
         <v>37</v>
@@ -3735,10 +3714,10 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C40" s="2">
         <v>38</v>
@@ -3782,10 +3761,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C41" s="2">
         <v>39</v>
@@ -3829,10 +3808,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>326</v>
+        <v>289</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>315</v>
       </c>
       <c r="C42" s="2">
         <v>40</v>
@@ -3876,10 +3855,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>323</v>
+        <v>289</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>319</v>
       </c>
       <c r="C43" s="2">
         <v>41</v>
@@ -3923,10 +3902,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C44" s="2">
         <v>42</v>
@@ -3970,10 +3949,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C45" s="2">
         <v>43</v>
@@ -4017,10 +3996,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="C46" s="2">
         <v>44</v>
@@ -4064,10 +4043,10 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C47" s="2">
         <v>45</v>
@@ -4110,11 +4089,11 @@
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>337</v>
+      <c r="A48" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>321</v>
       </c>
       <c r="C48" s="2">
         <v>46</v>
@@ -4158,10 +4137,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C49" s="2">
         <v>47</v>
@@ -4205,10 +4184,10 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C50" s="2">
         <v>48</v>
@@ -4252,10 +4231,10 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C51" s="2">
         <v>49</v>
@@ -4299,10 +4278,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C52" s="2">
         <v>50</v>
@@ -4346,10 +4325,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C53" s="2">
         <v>51</v>
@@ -4393,10 +4372,10 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C54" s="2">
         <v>52</v>
@@ -4440,10 +4419,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C55" s="2">
         <v>53</v>
@@ -4487,10 +4466,10 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C56" s="2">
         <v>54</v>
@@ -4534,10 +4513,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C57" s="2">
         <v>55</v>
@@ -4581,10 +4560,10 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C58" s="2">
         <v>56</v>
@@ -4628,10 +4607,10 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C59" s="2">
         <v>57</v>
@@ -4675,10 +4654,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>343</v>
       </c>
       <c r="C60" s="2">
         <v>58</v>
@@ -4722,10 +4701,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C61" s="2">
         <v>59</v>
@@ -4769,10 +4748,10 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C62" s="2">
         <v>60</v>
@@ -4816,10 +4795,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C63" s="2">
         <v>61</v>
@@ -4863,10 +4842,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C64" s="2">
         <v>62</v>
@@ -4910,10 +4889,10 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C65" s="2">
         <v>63</v>
@@ -4957,10 +4936,10 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="C66" s="2">
         <v>64</v>
@@ -5004,10 +4983,10 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C67" s="2">
         <v>65</v>
@@ -5051,10 +5030,10 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="C68" s="2">
         <v>66</v>
@@ -5098,10 +5077,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C69" s="2">
         <v>67</v>
@@ -5145,10 +5124,10 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C70" s="2">
         <v>68</v>
@@ -5192,10 +5171,10 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C71" s="2">
         <v>69</v>
@@ -5239,10 +5218,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="C72" s="2">
         <v>70</v>
@@ -5286,10 +5265,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C73" s="2">
         <v>71</v>
@@ -5333,10 +5312,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C74" s="2">
         <v>72</v>
@@ -5380,10 +5359,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C75" s="2">
         <v>73</v>
@@ -5427,10 +5406,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C76" s="2">
         <v>74</v>
@@ -5474,10 +5453,10 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="C77" s="2">
         <v>75</v>
@@ -5521,10 +5500,10 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C78" s="2">
         <v>76</v>
@@ -5568,10 +5547,10 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C79" s="2">
         <v>77</v>
@@ -5615,10 +5594,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C80" s="2">
         <v>78</v>
@@ -5662,10 +5641,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C81" s="2">
         <v>79</v>
@@ -5709,10 +5688,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C82" s="2">
         <v>80</v>
@@ -5756,10 +5735,10 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="C83" s="2">
         <v>81</v>
@@ -5803,10 +5782,10 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="C84" s="2">
         <v>82</v>
@@ -5850,10 +5829,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C85" s="2">
         <v>83</v>
@@ -5897,10 +5876,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="C86" s="2">
         <v>84</v>
@@ -5944,10 +5923,10 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C87" s="2">
         <v>85</v>
@@ -5991,10 +5970,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="C88" s="2">
         <v>86</v>
@@ -6038,10 +6017,10 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C89" s="2">
         <v>87</v>
@@ -6085,10 +6064,10 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="C90" s="2">
         <v>88</v>
@@ -6132,10 +6111,10 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C91" s="2">
         <v>89</v>
@@ -6179,10 +6158,10 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C92" s="2">
         <v>90</v>
@@ -6226,10 +6205,10 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C93" s="2">
         <v>91</v>
@@ -6273,10 +6252,10 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="C94" s="2">
         <v>92</v>
@@ -6320,10 +6299,10 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C95" s="2">
         <v>93</v>
@@ -6367,10 +6346,10 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="C96" s="2">
         <v>94</v>
@@ -6414,10 +6393,10 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C97" s="2">
         <v>95</v>
@@ -6461,10 +6440,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C98" s="2">
         <v>96</v>
@@ -6508,10 +6487,10 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C99" s="2">
         <v>97</v>
@@ -6555,10 +6534,10 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C100" s="2">
         <v>98</v>
@@ -6602,10 +6581,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="C101" s="2">
         <v>99</v>
@@ -6649,10 +6628,10 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C102" s="2">
         <v>100</v>
@@ -6696,10 +6675,10 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C103" s="2">
         <v>101</v>
@@ -6743,10 +6722,10 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C104" s="2">
         <v>102</v>
@@ -6790,10 +6769,10 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="C105" s="2">
         <v>103</v>
@@ -6836,10 +6815,10 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C106" s="2">
         <v>104</v>
@@ -6883,10 +6862,10 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="C107" s="2">
         <v>105</v>
@@ -6930,10 +6909,10 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="C108" s="2">
         <v>106</v>
@@ -6977,10 +6956,10 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="C109" s="2">
         <v>107</v>
@@ -7024,10 +7003,10 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="C110" s="2">
         <v>108</v>
@@ -7071,10 +7050,10 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C111" s="2">
         <v>109</v>
@@ -7118,10 +7097,10 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="C112" s="2">
         <v>110</v>
@@ -7165,10 +7144,10 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C113" s="2">
         <v>111</v>
@@ -7212,10 +7191,10 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C114" s="2">
         <v>112</v>
@@ -7259,10 +7238,10 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C115" s="2">
         <v>113</v>
@@ -7306,10 +7285,10 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="C116" s="2">
         <v>114</v>
@@ -7353,10 +7332,10 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="C117" s="2">
         <v>115</v>
@@ -7400,10 +7379,10 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="C118" s="2">
         <v>116</v>
@@ -7447,10 +7426,10 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C119" s="2">
         <v>117</v>
@@ -7494,10 +7473,10 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="C120" s="2">
         <v>118</v>
@@ -7541,10 +7520,10 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C121" s="2">
         <v>119</v>
@@ -7588,10 +7567,10 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C122" s="2">
         <v>120</v>
@@ -7635,10 +7614,10 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="C123" s="2">
         <v>121</v>
@@ -7682,10 +7661,10 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C124" s="2">
         <v>122</v>
@@ -7729,10 +7708,10 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C125" s="2">
         <v>123</v>
@@ -7776,10 +7755,10 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="C126" s="2">
         <v>124</v>
@@ -7823,10 +7802,10 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C127" s="2">
         <v>125</v>
@@ -7870,10 +7849,10 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C128" s="2">
         <v>126</v>
@@ -7917,10 +7896,10 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C129" s="2">
         <v>127</v>
@@ -7964,10 +7943,10 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C130" s="2">
         <v>128</v>
@@ -8011,10 +7990,10 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C131" s="2">
         <v>129</v>
@@ -8058,10 +8037,10 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C132" s="2">
         <v>130</v>
@@ -8105,10 +8084,10 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C133" s="2">
         <v>131</v>
@@ -8152,10 +8131,10 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C134" s="2">
         <v>132</v>
@@ -8199,10 +8178,10 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C135" s="2">
         <v>133</v>
@@ -8246,10 +8225,10 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C136" s="2">
         <v>134</v>
@@ -8293,10 +8272,10 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="C137" s="2">
         <v>135</v>
@@ -8340,10 +8319,10 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C138" s="2">
         <v>136</v>
@@ -8387,10 +8366,10 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="C139" s="2">
         <v>137</v>
@@ -8434,10 +8413,10 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C140" s="2">
         <v>138</v>
@@ -8481,10 +8460,10 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="C141" s="2">
         <v>139</v>
@@ -8528,10 +8507,10 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="C142" s="2">
         <v>140</v>
@@ -8575,10 +8554,10 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="C143" s="2">
         <v>141</v>
@@ -8622,10 +8601,10 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C144" s="2">
         <v>142</v>
@@ -8669,10 +8648,10 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="C145" s="2">
         <v>143</v>
@@ -8716,10 +8695,10 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="C146" s="2">
         <v>144</v>
@@ -8763,10 +8742,10 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C147" s="2">
         <v>145</v>
@@ -8810,10 +8789,10 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="C148" s="2">
         <v>146</v>
@@ -8857,10 +8836,10 @@
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="C149" s="2">
         <v>147</v>
@@ -8904,10 +8883,10 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="C150" s="2">
         <v>148</v>
@@ -8951,10 +8930,10 @@
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C151" s="2">
         <v>149</v>
@@ -8998,10 +8977,10 @@
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="C152" s="2">
         <v>150</v>
@@ -9045,10 +9024,10 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="C153" s="2">
         <v>151</v>
@@ -9092,10 +9071,10 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="C154" s="2">
         <v>152</v>
@@ -9139,10 +9118,10 @@
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="C155" s="2">
         <v>153</v>
@@ -9186,10 +9165,10 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C156" s="2">
         <v>154</v>
@@ -9233,10 +9212,10 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="C157" s="2">
         <v>155</v>
@@ -9280,10 +9259,10 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="C158" s="2">
         <v>156</v>
@@ -9327,10 +9306,10 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="C159" s="2">
         <v>157</v>
@@ -9374,10 +9353,10 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="C160" s="2">
         <v>158</v>
@@ -9421,10 +9400,10 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C161" s="2">
         <v>159</v>
@@ -9468,10 +9447,10 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="C162" s="2">
         <v>160</v>
@@ -9515,10 +9494,10 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B163" s="3" t="s">
         <v>440</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>447</v>
       </c>
       <c r="C163" s="2">
         <v>161</v>
@@ -9562,10 +9541,10 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="C164" s="2">
         <v>162</v>
@@ -9609,10 +9588,10 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="C165" s="2">
         <v>163</v>
@@ -9656,10 +9635,10 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="C166" s="2">
         <v>164</v>
@@ -9703,10 +9682,10 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C167" s="2">
         <v>165</v>
@@ -9750,10 +9729,10 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="C168" s="2">
         <v>166</v>
@@ -9797,10 +9776,10 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C169" s="2">
         <v>167</v>
@@ -9844,10 +9823,10 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="C170" s="2">
         <v>168</v>
@@ -9891,10 +9870,10 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C171" s="2">
         <v>169</v>
@@ -9938,10 +9917,10 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C172" s="2">
         <v>170</v>
@@ -9985,10 +9964,10 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C173" s="2">
         <v>171</v>
@@ -10032,10 +10011,10 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C174" s="2">
         <v>172</v>
@@ -10079,10 +10058,10 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="C175" s="2">
         <v>173</v>
@@ -10126,10 +10105,10 @@
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="C176" s="2">
         <v>174</v>
@@ -10173,10 +10152,10 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C177" s="2">
         <v>175</v>
@@ -10220,10 +10199,10 @@
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="C178" s="2">
         <v>176</v>
@@ -10267,10 +10246,10 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C179" s="2">
         <v>177</v>
@@ -10314,10 +10293,10 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="C180" s="2">
         <v>178</v>
@@ -10361,10 +10340,10 @@
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="C181" s="2">
         <v>179</v>
@@ -10408,10 +10387,10 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="C182" s="2">
         <v>180</v>
@@ -10455,10 +10434,10 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C183" s="2">
         <v>181</v>
@@ -10502,10 +10481,10 @@
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C184" s="2">
         <v>182</v>
@@ -10549,10 +10528,10 @@
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C185" s="2">
         <v>183</v>
@@ -10596,10 +10575,10 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" s="8" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C186" s="2">
         <v>184</v>
@@ -10643,10 +10622,10 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C187" s="2">
         <v>185</v>
@@ -10690,10 +10669,10 @@
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>329</v>
+        <v>470</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C188" s="2">
         <v>186</v>
@@ -10737,10 +10716,10 @@
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>329</v>
+        <v>470</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C189" s="2">
         <v>187</v>
@@ -10784,10 +10763,10 @@
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
-        <v>329</v>
+        <v>470</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C190" s="2">
         <v>188</v>
@@ -10831,10 +10810,10 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
-        <v>329</v>
+        <v>470</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C191" s="2">
         <v>189</v>
@@ -10878,10 +10857,10 @@
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
-        <v>329</v>
+        <v>470</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C192" s="2">
         <v>190</v>
@@ -10925,10 +10904,10 @@
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
-        <v>329</v>
+        <v>470</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C193" s="2">
         <v>191</v>
@@ -10972,10 +10951,10 @@
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C194" s="2">
         <v>192</v>
@@ -11019,9 +10998,11 @@
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B195" s="2"/>
+        <v>465</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="C195" s="2">
         <v>193</v>
       </c>
@@ -11064,9 +11045,11 @@
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B196" s="2"/>
+        <v>465</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>467</v>
+      </c>
       <c r="C196" s="2">
         <v>194</v>
       </c>
@@ -11109,9 +11092,11 @@
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B197" s="2"/>
+        <v>465</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>468</v>
+      </c>
       <c r="C197" s="2">
         <v>195</v>
       </c>
@@ -11154,9 +11139,11 @@
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B198" s="2"/>
+        <v>465</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>469</v>
+      </c>
       <c r="C198" s="2">
         <v>196</v>
       </c>
@@ -11199,9 +11186,11 @@
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B199" s="2"/>
+        <v>465</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>321</v>
+      </c>
       <c r="C199" s="2">
         <v>197</v>
       </c>
@@ -11244,10 +11233,10 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C200" s="2">
         <v>198</v>
@@ -11291,10 +11280,10 @@
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C201" s="2">
         <v>199</v>
@@ -11338,10 +11327,10 @@
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C202" s="2">
         <v>200</v>
@@ -11385,10 +11374,10 @@
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C203" s="2">
         <v>201</v>
@@ -11432,10 +11421,10 @@
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C204" s="2">
         <v>202</v>
@@ -11479,10 +11468,10 @@
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C205" s="2">
         <v>203</v>
@@ -11526,10 +11515,10 @@
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C206" s="2">
         <v>204</v>
@@ -11573,10 +11562,10 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C207" s="2">
         <v>205</v>
@@ -11620,10 +11609,10 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C208" s="2">
         <v>206</v>
@@ -11667,10 +11656,10 @@
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C209" s="2">
         <v>207</v>
@@ -11714,10 +11703,10 @@
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C210" s="2">
         <v>208</v>
@@ -11761,10 +11750,10 @@
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C211" s="2">
         <v>209</v>
@@ -11808,10 +11797,10 @@
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C212" s="2">
         <v>210</v>
@@ -11855,10 +11844,10 @@
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C213" s="2">
         <v>211</v>
@@ -11902,10 +11891,10 @@
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="C214" s="2">
         <v>212</v>
@@ -11949,10 +11938,10 @@
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C215" s="2">
         <v>213</v>
@@ -11996,10 +11985,10 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="C216" s="2">
         <v>214</v>
@@ -12043,10 +12032,10 @@
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="C217" s="2">
         <v>215</v>
@@ -12087,7 +12076,7 @@
         <v>229</v>
       </c>
       <c r="M217" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First push of AcceptMap
</commit_message>
<xml_diff>
--- a/fMRI Tasks/info/biopac_code_dict.xlsx
+++ b/fMRI Tasks/info/biopac_code_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C4FA63-28BA-42AE-A310-3109ABD91141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704DAF0-C86B-4A8D-AD9A-4624E6F78171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="285" windowWidth="38640" windowHeight="22650" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
+    <workbookView xWindow="-18120" yWindow="285" windowWidth="18240" windowHeight="27450" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="474">
   <si>
     <t>D8</t>
   </si>
@@ -858,57 +858,12 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>affect_rating</t>
-  </si>
-  <si>
-    <t>post_outcome_fixation_start</t>
-  </si>
-  <si>
-    <t>pair_start_med_low</t>
-  </si>
-  <si>
-    <t>pair_start_med_high</t>
-  </si>
-  <si>
-    <t>pair_start_med_gain</t>
-  </si>
-  <si>
-    <t>pair_start_med_loss</t>
-  </si>
-  <si>
-    <t>outcome_start_med</t>
-  </si>
-  <si>
-    <t>outcome_start_low</t>
-  </si>
-  <si>
-    <t>outcome_start_high</t>
-  </si>
-  <si>
-    <t>outcome_start_gain</t>
-  </si>
-  <si>
-    <t>outcome_start_loss</t>
-  </si>
-  <si>
-    <t>gain_outcome_start</t>
-  </si>
-  <si>
-    <t>loss_outcome_start</t>
-  </si>
-  <si>
-    <t>lottary_start</t>
-  </si>
-  <si>
     <t>imagination_instruction</t>
   </si>
   <si>
     <t>bodymapping</t>
   </si>
   <si>
-    <t>expectancy_distraction</t>
-  </si>
-  <si>
     <t>hyperalignment</t>
   </si>
   <si>
@@ -1449,10 +1404,58 @@
     <t>t1_test/distractmap</t>
   </si>
   <si>
-    <t>bodymapping/distractmap</t>
-  </si>
-  <si>
     <t>bodymapping_instruction</t>
+  </si>
+  <si>
+    <t>experience_instructions</t>
+  </si>
+  <si>
+    <t>regulate_instructions</t>
+  </si>
+  <si>
+    <t>avoid_rating_start</t>
+  </si>
+  <si>
+    <t>relax_rating_start</t>
+  </si>
+  <si>
+    <t>taskattention_rating_start</t>
+  </si>
+  <si>
+    <t>boredom_rating_start</t>
+  </si>
+  <si>
+    <t>alertness_rating_start</t>
+  </si>
+  <si>
+    <t>posthx_rating_start</t>
+  </si>
+  <si>
+    <t>negthx_rating_start</t>
+  </si>
+  <si>
+    <t>self_rating_start</t>
+  </si>
+  <si>
+    <t>other_rating_start</t>
+  </si>
+  <si>
+    <t>imagery_rating_start</t>
+  </si>
+  <si>
+    <t>present_rating_start</t>
+  </si>
+  <si>
+    <t>bodymapping/distractmap/acceptmap</t>
+  </si>
+  <si>
+    <t>acceptmap_regulate</t>
+  </si>
+  <si>
+    <t>acceptmap_preexperience</t>
+  </si>
+  <si>
+    <t>acceptmap_postexperience</t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31222A2-51DB-244C-8B3D-C257DC9A15AB}">
   <dimension ref="A1:N268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="E208" sqref="E208"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1992,7 +1995,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>13</v>
@@ -2039,7 +2042,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>13</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>13</v>
@@ -2133,7 +2136,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>13</v>
@@ -2179,9 +2182,7 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>465</v>
-      </c>
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2228,7 +2229,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -2276,7 +2277,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>13</v>
@@ -2323,8 +2324,12 @@
       <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C10" s="2">
         <v>8</v>
       </c>
@@ -2367,8 +2372,12 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C11" s="2">
         <v>9</v>
       </c>
@@ -2411,8 +2420,12 @@
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C12" s="2">
         <v>10</v>
       </c>
@@ -2586,7 +2599,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>271</v>
@@ -2632,11 +2645,11 @@
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>471</v>
+      <c r="A17" s="8" t="s">
+        <v>470</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="C17" s="2">
         <v>15</v>
@@ -2680,10 +2693,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C18" s="2">
         <v>16</v>
@@ -2727,10 +2740,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C19" s="2">
         <v>17</v>
@@ -2774,10 +2787,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C20" s="2">
         <v>18</v>
@@ -2821,10 +2834,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C21" s="2">
         <v>19</v>
@@ -2868,10 +2881,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C22" s="2">
         <v>20</v>
@@ -2915,10 +2928,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="C23" s="2">
         <v>21</v>
@@ -2962,10 +2975,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="C24" s="2">
         <v>22</v>
@@ -3009,10 +3022,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C25" s="2">
         <v>23</v>
@@ -3056,10 +3069,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="C26" s="2">
         <v>24</v>
@@ -3103,10 +3116,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C27" s="2">
         <v>25</v>
@@ -3150,10 +3163,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C28" s="2">
         <v>26</v>
@@ -3197,10 +3210,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="C29" s="2">
         <v>27</v>
@@ -3244,10 +3257,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="C30" s="2">
         <v>28</v>
@@ -3291,10 +3304,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>289</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="C31" s="2">
         <v>29</v>
@@ -3338,10 +3351,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="C32" s="2">
         <v>30</v>
@@ -3385,10 +3398,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="C33" s="2">
         <v>31</v>
@@ -3432,10 +3445,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C34" s="2">
         <v>32</v>
@@ -3479,10 +3492,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="C35" s="2">
         <v>33</v>
@@ -3526,10 +3539,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="C36" s="2">
         <v>34</v>
@@ -3573,10 +3586,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="C37" s="2">
         <v>35</v>
@@ -3620,10 +3633,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="C38" s="2">
         <v>36</v>
@@ -3667,10 +3680,10 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="C39" s="2">
         <v>37</v>
@@ -3714,10 +3727,10 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="C40" s="2">
         <v>38</v>
@@ -3761,10 +3774,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C41" s="2">
         <v>39</v>
@@ -3808,10 +3821,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="C42" s="2">
         <v>40</v>
@@ -3855,10 +3868,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C43" s="2">
         <v>41</v>
@@ -3902,10 +3915,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C44" s="2">
         <v>42</v>
@@ -3949,10 +3962,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="C45" s="2">
         <v>43</v>
@@ -3996,10 +4009,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="C46" s="2">
         <v>44</v>
@@ -4043,10 +4056,10 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="C47" s="2">
         <v>45</v>
@@ -4090,10 +4103,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C48" s="2">
         <v>46</v>
@@ -4137,10 +4150,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C49" s="2">
         <v>47</v>
@@ -4184,10 +4197,10 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C50" s="2">
         <v>48</v>
@@ -4231,10 +4244,10 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C51" s="2">
         <v>49</v>
@@ -4278,10 +4291,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C52" s="2">
         <v>50</v>
@@ -4325,10 +4338,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C53" s="2">
         <v>51</v>
@@ -4372,10 +4385,10 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C54" s="2">
         <v>52</v>
@@ -4419,10 +4432,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="C55" s="2">
         <v>53</v>
@@ -4466,10 +4479,10 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C56" s="2">
         <v>54</v>
@@ -4513,10 +4526,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C57" s="2">
         <v>55</v>
@@ -4560,10 +4573,10 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="C58" s="2">
         <v>56</v>
@@ -4607,10 +4620,10 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="C59" s="2">
         <v>57</v>
@@ -4654,10 +4667,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C60" s="2">
         <v>58</v>
@@ -4701,10 +4714,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="C61" s="2">
         <v>59</v>
@@ -4748,10 +4761,10 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="C62" s="2">
         <v>60</v>
@@ -4795,10 +4808,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="C63" s="2">
         <v>61</v>
@@ -4842,10 +4855,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C64" s="2">
         <v>62</v>
@@ -4889,10 +4902,10 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C65" s="2">
         <v>63</v>
@@ -4936,10 +4949,10 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C66" s="2">
         <v>64</v>
@@ -4983,10 +4996,10 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="C67" s="2">
         <v>65</v>
@@ -5030,10 +5043,10 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>344</v>
       </c>
       <c r="C68" s="2">
         <v>66</v>
@@ -5077,10 +5090,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="C69" s="2">
         <v>67</v>
@@ -5124,10 +5137,10 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C70" s="2">
         <v>68</v>
@@ -5171,10 +5184,10 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C71" s="2">
         <v>69</v>
@@ -5218,10 +5231,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C72" s="2">
         <v>70</v>
@@ -5265,10 +5278,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C73" s="2">
         <v>71</v>
@@ -5312,10 +5325,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C74" s="2">
         <v>72</v>
@@ -5359,10 +5372,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C75" s="2">
         <v>73</v>
@@ -5406,10 +5419,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="C76" s="2">
         <v>74</v>
@@ -5453,10 +5466,10 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="C77" s="2">
         <v>75</v>
@@ -5500,10 +5513,10 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C78" s="2">
         <v>76</v>
@@ -5547,10 +5560,10 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C79" s="2">
         <v>77</v>
@@ -5594,10 +5607,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="C80" s="2">
         <v>78</v>
@@ -5641,10 +5654,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C81" s="2">
         <v>79</v>
@@ -5688,10 +5701,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C82" s="2">
         <v>80</v>
@@ -5735,10 +5748,10 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C83" s="2">
         <v>81</v>
@@ -5782,10 +5795,10 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C84" s="2">
         <v>82</v>
@@ -5829,10 +5842,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="C85" s="2">
         <v>83</v>
@@ -5876,10 +5889,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="C86" s="2">
         <v>84</v>
@@ -5923,10 +5936,10 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="C87" s="2">
         <v>85</v>
@@ -5970,10 +5983,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="C88" s="2">
         <v>86</v>
@@ -6017,10 +6030,10 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="C89" s="2">
         <v>87</v>
@@ -6064,10 +6077,10 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="C90" s="2">
         <v>88</v>
@@ -6111,10 +6124,10 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="C91" s="2">
         <v>89</v>
@@ -6158,10 +6171,10 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="C92" s="2">
         <v>90</v>
@@ -6205,10 +6218,10 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="C93" s="2">
         <v>91</v>
@@ -6252,10 +6265,10 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="C94" s="2">
         <v>92</v>
@@ -6299,10 +6312,10 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="C95" s="2">
         <v>93</v>
@@ -6346,10 +6359,10 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="C96" s="2">
         <v>94</v>
@@ -6393,10 +6406,10 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="C97" s="2">
         <v>95</v>
@@ -6440,10 +6453,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="C98" s="2">
         <v>96</v>
@@ -6487,10 +6500,10 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="C99" s="2">
         <v>97</v>
@@ -6534,10 +6547,10 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="C100" s="2">
         <v>98</v>
@@ -6581,10 +6594,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="C101" s="2">
         <v>99</v>
@@ -6628,10 +6641,10 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="C102" s="2">
         <v>100</v>
@@ -6675,10 +6688,10 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="C103" s="2">
         <v>101</v>
@@ -6722,10 +6735,10 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="C104" s="2">
         <v>102</v>
@@ -6769,10 +6782,10 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="C105" s="2">
         <v>103</v>
@@ -6815,10 +6828,10 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="C106" s="2">
         <v>104</v>
@@ -6862,10 +6875,10 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="C107" s="2">
         <v>105</v>
@@ -6909,10 +6922,10 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="C108" s="2">
         <v>106</v>
@@ -6956,10 +6969,10 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="C109" s="2">
         <v>107</v>
@@ -7003,10 +7016,10 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="C110" s="2">
         <v>108</v>
@@ -7050,10 +7063,10 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="C111" s="2">
         <v>109</v>
@@ -7097,10 +7110,10 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="C112" s="2">
         <v>110</v>
@@ -7144,10 +7157,10 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="C113" s="2">
         <v>111</v>
@@ -7191,10 +7204,10 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="C114" s="2">
         <v>112</v>
@@ -7238,10 +7251,10 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="C115" s="2">
         <v>113</v>
@@ -7285,10 +7298,10 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="C116" s="2">
         <v>114</v>
@@ -7332,10 +7345,10 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="C117" s="2">
         <v>115</v>
@@ -7379,10 +7392,10 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="C118" s="2">
         <v>116</v>
@@ -7426,10 +7439,10 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="C119" s="2">
         <v>117</v>
@@ -7473,10 +7486,10 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="C120" s="2">
         <v>118</v>
@@ -7520,10 +7533,10 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="C121" s="2">
         <v>119</v>
@@ -7567,10 +7580,10 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="C122" s="2">
         <v>120</v>
@@ -7614,10 +7627,10 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="C123" s="2">
         <v>121</v>
@@ -7661,10 +7674,10 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="C124" s="2">
         <v>122</v>
@@ -7708,10 +7721,10 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="C125" s="2">
         <v>123</v>
@@ -7755,10 +7768,10 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="C126" s="2">
         <v>124</v>
@@ -7802,10 +7815,10 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="C127" s="2">
         <v>125</v>
@@ -7849,10 +7862,10 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C128" s="2">
         <v>126</v>
@@ -7896,10 +7909,10 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="C129" s="2">
         <v>127</v>
@@ -7943,10 +7956,10 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="C130" s="2">
         <v>128</v>
@@ -7990,10 +8003,10 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="C131" s="2">
         <v>129</v>
@@ -8037,10 +8050,10 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="C132" s="2">
         <v>130</v>
@@ -8084,10 +8097,10 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="C133" s="2">
         <v>131</v>
@@ -8131,10 +8144,10 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="C134" s="2">
         <v>132</v>
@@ -8178,10 +8191,10 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="C135" s="2">
         <v>133</v>
@@ -8225,10 +8238,10 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="C136" s="2">
         <v>134</v>
@@ -8272,10 +8285,10 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="C137" s="2">
         <v>135</v>
@@ -8319,10 +8332,10 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="C138" s="2">
         <v>136</v>
@@ -8366,10 +8379,10 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="C139" s="2">
         <v>137</v>
@@ -8413,10 +8426,10 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="C140" s="2">
         <v>138</v>
@@ -8460,10 +8473,10 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="C141" s="2">
         <v>139</v>
@@ -8507,10 +8520,10 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="C142" s="2">
         <v>140</v>
@@ -8554,10 +8567,10 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C143" s="2">
         <v>141</v>
@@ -8601,10 +8614,10 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="C144" s="2">
         <v>142</v>
@@ -8648,10 +8661,10 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="C145" s="2">
         <v>143</v>
@@ -8695,10 +8708,10 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="C146" s="2">
         <v>144</v>
@@ -8742,10 +8755,10 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="C147" s="2">
         <v>145</v>
@@ -8789,10 +8802,10 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="C148" s="2">
         <v>146</v>
@@ -8836,10 +8849,10 @@
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="C149" s="2">
         <v>147</v>
@@ -8883,10 +8896,10 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="C150" s="2">
         <v>148</v>
@@ -8930,10 +8943,10 @@
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="C151" s="2">
         <v>149</v>
@@ -8977,10 +8990,10 @@
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="C152" s="2">
         <v>150</v>
@@ -9024,10 +9037,10 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="C153" s="2">
         <v>151</v>
@@ -9071,10 +9084,10 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="C154" s="2">
         <v>152</v>
@@ -9118,10 +9131,10 @@
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="C155" s="2">
         <v>153</v>
@@ -9165,10 +9178,10 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C156" s="2">
         <v>154</v>
@@ -9212,10 +9225,10 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="C157" s="2">
         <v>155</v>
@@ -9259,10 +9272,10 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="C158" s="2">
         <v>156</v>
@@ -9306,10 +9319,10 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="C159" s="2">
         <v>157</v>
@@ -9353,10 +9366,10 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="C160" s="2">
         <v>158</v>
@@ -9400,10 +9413,10 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="C161" s="2">
         <v>159</v>
@@ -9447,10 +9460,10 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="C162" s="2">
         <v>160</v>
@@ -9494,10 +9507,10 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="C163" s="2">
         <v>161</v>
@@ -9541,10 +9554,10 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="C164" s="2">
         <v>162</v>
@@ -9588,10 +9601,10 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="C165" s="2">
         <v>163</v>
@@ -9635,10 +9648,10 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="C166" s="2">
         <v>164</v>
@@ -9682,10 +9695,10 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="C167" s="2">
         <v>165</v>
@@ -9729,10 +9742,10 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="C168" s="2">
         <v>166</v>
@@ -9776,10 +9789,10 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="C169" s="2">
         <v>167</v>
@@ -9823,10 +9836,10 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="C170" s="2">
         <v>168</v>
@@ -9870,10 +9883,10 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B171" s="3" t="s">
         <v>433</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>448</v>
       </c>
       <c r="C171" s="2">
         <v>169</v>
@@ -9917,10 +9930,10 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="C172" s="2">
         <v>170</v>
@@ -9964,10 +9977,10 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="C173" s="2">
         <v>171</v>
@@ -10011,10 +10024,10 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="C174" s="2">
         <v>172</v>
@@ -10058,10 +10071,10 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C175" s="2">
         <v>173</v>
@@ -10105,10 +10118,10 @@
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="C176" s="2">
         <v>174</v>
@@ -10152,10 +10165,10 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C177" s="2">
         <v>175</v>
@@ -10199,10 +10212,10 @@
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="C178" s="2">
         <v>176</v>
@@ -10246,10 +10259,10 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="C179" s="2">
         <v>177</v>
@@ -10293,10 +10306,10 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="C180" s="2">
         <v>178</v>
@@ -10340,10 +10353,10 @@
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="C181" s="2">
         <v>179</v>
@@ -10387,10 +10400,10 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="C182" s="2">
         <v>180</v>
@@ -10434,10 +10447,10 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="C183" s="2">
         <v>181</v>
@@ -10481,10 +10494,10 @@
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="C184" s="2">
         <v>182</v>
@@ -10528,10 +10541,10 @@
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="C185" s="2">
         <v>183</v>
@@ -10575,7 +10588,7 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" s="8" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B186" s="10" t="s">
         <v>271</v>
@@ -10622,10 +10635,10 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="C187" s="2">
         <v>185</v>
@@ -10669,10 +10682,10 @@
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="C188" s="2">
         <v>186</v>
@@ -10716,10 +10729,10 @@
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="C189" s="2">
         <v>187</v>
@@ -10763,10 +10776,10 @@
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C190" s="2">
         <v>188</v>
@@ -10810,10 +10823,10 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="C191" s="2">
         <v>189</v>
@@ -10857,10 +10870,10 @@
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="C192" s="2">
         <v>190</v>
@@ -10904,10 +10917,10 @@
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="C193" s="2">
         <v>191</v>
@@ -10951,10 +10964,10 @@
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C194" s="2">
         <v>192</v>
@@ -10998,7 +11011,7 @@
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>271</v>
@@ -11045,10 +11058,10 @@
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="C196" s="2">
         <v>194</v>
@@ -11092,10 +11105,10 @@
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="C197" s="2">
         <v>195</v>
@@ -11139,10 +11152,10 @@
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="C198" s="2">
         <v>196</v>
@@ -11186,10 +11199,10 @@
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C199" s="2">
         <v>197</v>
@@ -11233,10 +11246,10 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>276</v>
+        <v>457</v>
       </c>
       <c r="C200" s="2">
         <v>198</v>
@@ -11280,10 +11293,10 @@
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>277</v>
+        <v>458</v>
       </c>
       <c r="C201" s="2">
         <v>199</v>
@@ -11327,10 +11340,10 @@
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>278</v>
+        <v>459</v>
       </c>
       <c r="C202" s="2">
         <v>200</v>
@@ -11374,10 +11387,10 @@
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>279</v>
+        <v>460</v>
       </c>
       <c r="C203" s="2">
         <v>201</v>
@@ -11421,10 +11434,10 @@
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>287</v>
+        <v>461</v>
       </c>
       <c r="C204" s="2">
         <v>202</v>
@@ -11468,10 +11481,10 @@
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>280</v>
+        <v>462</v>
       </c>
       <c r="C205" s="2">
         <v>203</v>
@@ -11515,10 +11528,10 @@
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>281</v>
+        <v>463</v>
       </c>
       <c r="C206" s="2">
         <v>204</v>
@@ -11562,10 +11575,10 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>282</v>
+        <v>464</v>
       </c>
       <c r="C207" s="2">
         <v>205</v>
@@ -11609,10 +11622,10 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>283</v>
+        <v>465</v>
       </c>
       <c r="C208" s="2">
         <v>206</v>
@@ -11656,10 +11669,10 @@
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>284</v>
+        <v>466</v>
       </c>
       <c r="C209" s="2">
         <v>207</v>
@@ -11703,10 +11716,10 @@
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>275</v>
+        <v>467</v>
       </c>
       <c r="C210" s="2">
         <v>208</v>
@@ -11750,10 +11763,10 @@
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>274</v>
+        <v>468</v>
       </c>
       <c r="C211" s="2">
         <v>209</v>
@@ -11797,10 +11810,10 @@
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" s="8" t="s">
-        <v>290</v>
+        <v>451</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>285</v>
+        <v>469</v>
       </c>
       <c r="C212" s="2">
         <v>210</v>
@@ -11843,12 +11856,8 @@
       <c r="M212" s="2"/>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A213" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="B213" s="8" t="s">
-        <v>286</v>
-      </c>
+      <c r="A213" s="8"/>
+      <c r="B213" s="8"/>
       <c r="C213" s="2">
         <v>211</v>
       </c>
@@ -11891,10 +11900,10 @@
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" s="8" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="C214" s="2">
         <v>212</v>
@@ -11938,10 +11947,10 @@
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" s="8" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="C215" s="2">
         <v>213</v>
@@ -11985,10 +11994,10 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" s="8" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="C216" s="2">
         <v>214</v>
@@ -12032,10 +12041,10 @@
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" s="8" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="C217" s="2">
         <v>215</v>
@@ -12083,6 +12092,7 @@
       <c r="A218" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B218" s="2"/>
       <c r="C218" s="2">
         <v>216</v>
       </c>

</xml_diff>